<commit_message>
adding excel file for saxpy DGPU 0 0
</commit_message>
<xml_diff>
--- a/Measures/data_convolution_DGPU_0_0.xlsx
+++ b/Measures/data_convolution_DGPU_0_0.xlsx
@@ -2205,8 +2205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N1" activeCellId="1" sqref="E1:E10 N1:N10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>